<commit_message>
more incorrect constraints identified
SE10 - SE13
</commit_message>
<xml_diff>
--- a/solution.xlsx
+++ b/solution.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B118"/>
+  <dimension ref="A1:B107"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,7 +443,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>R_ij_t[1,5,1]</t>
+          <t>R_ij_t[1,3,2]</t>
         </is>
       </c>
       <c r="B2" t="n">
@@ -453,7 +453,7 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>R_ij_t[2,6,2]</t>
+          <t>R_ij_t[2,4,1]</t>
         </is>
       </c>
       <c r="B3" t="n">
@@ -463,7 +463,7 @@
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>R_ij_t[3,1,1]</t>
+          <t>R_ij_t[3,5,2]</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -473,7 +473,7 @@
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>R_ij_t[4,2,2]</t>
+          <t>R_ij_t[4,6,1]</t>
         </is>
       </c>
       <c r="B5" t="n">
@@ -483,7 +483,7 @@
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>R_ij_t[5,3,1]</t>
+          <t>R_ij_t[5,1,2]</t>
         </is>
       </c>
       <c r="B6" t="n">
@@ -493,7 +493,7 @@
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>R_ij_t[6,4,2]</t>
+          <t>R_ij_t[6,2,1]</t>
         </is>
       </c>
       <c r="B7" t="n">
@@ -543,7 +543,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>X_ij_v[3,10,6]</t>
+          <t>X_ij_v[3,14,5]</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -593,7 +593,7 @@
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>X_ij_v[4,11,4]</t>
+          <t>X_ij_v[4,9,6]</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -643,7 +643,7 @@
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>X_ij_v[5,12,5]</t>
+          <t>X_ij_v[5,18,4]</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -693,7 +693,7 @@
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>X_ij_v[6,7,3]</t>
+          <t>X_ij_v[6,15,3]</t>
         </is>
       </c>
       <c r="B27" t="n">
@@ -703,7 +703,7 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>X_ij_v[7,17,3]</t>
+          <t>X_ij_v[7,6,3]</t>
         </is>
       </c>
       <c r="B28" t="n">
@@ -713,7 +713,7 @@
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>X_ij_v[8,14,6]</t>
+          <t>X_ij_v[8,10,5]</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -723,7 +723,7 @@
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>X_ij_v[9,4,4]</t>
+          <t>X_ij_v[9,13,6]</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -733,7 +733,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>X_ij_v[10,8,6]</t>
+          <t>X_ij_v[10,3,5]</t>
         </is>
       </c>
       <c r="B31" t="n">
@@ -743,7 +743,7 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>X_ij_v[11,13,4]</t>
+          <t>X_ij_v[11,4,6]</t>
         </is>
       </c>
       <c r="B32" t="n">
@@ -753,7 +753,7 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>X_ij_v[12,16,5]</t>
+          <t>X_ij_v[12,5,4]</t>
         </is>
       </c>
       <c r="B33" t="n">
@@ -763,7 +763,7 @@
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>X_ij_v[13,9,4]</t>
+          <t>X_ij_v[13,11,6]</t>
         </is>
       </c>
       <c r="B34" t="n">
@@ -773,7 +773,7 @@
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>X_ij_v[14,3,6]</t>
+          <t>X_ij_v[14,8,5]</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -783,7 +783,7 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>X_ij_v[15,6,3]</t>
+          <t>X_ij_v[15,17,3]</t>
         </is>
       </c>
       <c r="B36" t="n">
@@ -793,7 +793,7 @@
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>X_ij_v[16,18,5]</t>
+          <t>X_ij_v[16,12,4]</t>
         </is>
       </c>
       <c r="B37" t="n">
@@ -803,7 +803,7 @@
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>X_ij_v[17,15,3]</t>
+          <t>X_ij_v[17,7,3]</t>
         </is>
       </c>
       <c r="B38" t="n">
@@ -813,7 +813,7 @@
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>X_ij_v[18,5,5]</t>
+          <t>X_ij_v[18,16,4]</t>
         </is>
       </c>
       <c r="B39" t="n">
@@ -883,7 +883,7 @@
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>Y_c_t[7,2]</t>
+          <t>Y_c_t[7,1]</t>
         </is>
       </c>
       <c r="B46" t="n">
@@ -893,7 +893,7 @@
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>Y_c_t[8,1]</t>
+          <t>Y_c_t[8,2]</t>
         </is>
       </c>
       <c r="B47" t="n">
@@ -903,7 +903,7 @@
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>Y_c_t[9,2]</t>
+          <t>Y_c_t[9,1]</t>
         </is>
       </c>
       <c r="B48" t="n">
@@ -913,7 +913,7 @@
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>Y_c_t[10,1]</t>
+          <t>Y_c_t[10,2]</t>
         </is>
       </c>
       <c r="B49" t="n">
@@ -923,7 +923,7 @@
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>Y_c_t[11,2]</t>
+          <t>Y_c_t[11,1]</t>
         </is>
       </c>
       <c r="B50" t="n">
@@ -933,7 +933,7 @@
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>Y_c_t[12,1]</t>
+          <t>Y_c_t[12,2]</t>
         </is>
       </c>
       <c r="B51" t="n">
@@ -943,7 +943,7 @@
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>Y_c_t[13,2]</t>
+          <t>Y_c_t[13,1]</t>
         </is>
       </c>
       <c r="B52" t="n">
@@ -953,7 +953,7 @@
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>Y_c_t[14,1]</t>
+          <t>Y_c_t[14,2]</t>
         </is>
       </c>
       <c r="B53" t="n">
@@ -963,7 +963,7 @@
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>Y_c_t[15,2]</t>
+          <t>Y_c_t[15,1]</t>
         </is>
       </c>
       <c r="B54" t="n">
@@ -973,7 +973,7 @@
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>Y_c_t[16,1]</t>
+          <t>Y_c_t[16,2]</t>
         </is>
       </c>
       <c r="B55" t="n">
@@ -983,7 +983,7 @@
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>Y_c_t[17,2]</t>
+          <t>Y_c_t[17,1]</t>
         </is>
       </c>
       <c r="B56" t="n">
@@ -993,7 +993,7 @@
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>Y_c_t[18,1]</t>
+          <t>Y_c_t[18,2]</t>
         </is>
       </c>
       <c r="B57" t="n">
@@ -1013,7 +1013,7 @@
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>Y_c_v[8,6]</t>
+          <t>Y_c_v[8,5]</t>
         </is>
       </c>
       <c r="B59" t="n">
@@ -1023,7 +1023,7 @@
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>Y_c_v[9,4]</t>
+          <t>Y_c_v[9,6]</t>
         </is>
       </c>
       <c r="B60" t="n">
@@ -1033,7 +1033,7 @@
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>Y_c_v[10,6]</t>
+          <t>Y_c_v[10,5]</t>
         </is>
       </c>
       <c r="B61" t="n">
@@ -1043,7 +1043,7 @@
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>Y_c_v[11,4]</t>
+          <t>Y_c_v[11,6]</t>
         </is>
       </c>
       <c r="B62" t="n">
@@ -1053,7 +1053,7 @@
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>Y_c_v[12,5]</t>
+          <t>Y_c_v[12,4]</t>
         </is>
       </c>
       <c r="B63" t="n">
@@ -1063,7 +1063,7 @@
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>Y_c_v[13,4]</t>
+          <t>Y_c_v[13,6]</t>
         </is>
       </c>
       <c r="B64" t="n">
@@ -1073,7 +1073,7 @@
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>Y_c_v[14,6]</t>
+          <t>Y_c_v[14,5]</t>
         </is>
       </c>
       <c r="B65" t="n">
@@ -1093,7 +1093,7 @@
     <row r="67">
       <c r="A67" s="1" t="inlineStr">
         <is>
-          <t>Y_c_v[16,5]</t>
+          <t>Y_c_v[16,4]</t>
         </is>
       </c>
       <c r="B67" t="n">
@@ -1113,7 +1113,7 @@
     <row r="69">
       <c r="A69" s="1" t="inlineStr">
         <is>
-          <t>Y_c_v[18,5]</t>
+          <t>Y_c_v[18,4]</t>
         </is>
       </c>
       <c r="B69" t="n">
@@ -1253,7 +1253,7 @@
     <row r="83">
       <c r="A83" s="1" t="inlineStr">
         <is>
-          <t>B_v_s[4,4]</t>
+          <t>B_v_s[4,5]</t>
         </is>
       </c>
       <c r="B83" t="n">
@@ -1263,7 +1263,7 @@
     <row r="84">
       <c r="A84" s="1" t="inlineStr">
         <is>
-          <t>B_v_s[5,5]</t>
+          <t>B_v_s[5,3]</t>
         </is>
       </c>
       <c r="B84" t="n">
@@ -1273,7 +1273,7 @@
     <row r="85">
       <c r="A85" s="1" t="inlineStr">
         <is>
-          <t>B_v_s[6,3]</t>
+          <t>B_v_s[6,4]</t>
         </is>
       </c>
       <c r="B85" t="n">
@@ -1283,7 +1283,7 @@
     <row r="86">
       <c r="A86" s="1" t="inlineStr">
         <is>
-          <t>H_ij_v[3,10,6]</t>
+          <t>H_ij_v[3,14,5]</t>
         </is>
       </c>
       <c r="B86" t="n">
@@ -1293,7 +1293,7 @@
     <row r="87">
       <c r="A87" s="1" t="inlineStr">
         <is>
-          <t>H_ij_v[4,11,4]</t>
+          <t>H_ij_v[4,9,6]</t>
         </is>
       </c>
       <c r="B87" t="n">
@@ -1303,7 +1303,7 @@
     <row r="88">
       <c r="A88" s="1" t="inlineStr">
         <is>
-          <t>H_ij_v[5,12,5]</t>
+          <t>H_ij_v[5,18,4]</t>
         </is>
       </c>
       <c r="B88" t="n">
@@ -1313,7 +1313,7 @@
     <row r="89">
       <c r="A89" s="1" t="inlineStr">
         <is>
-          <t>H_ij_v[6,7,3]</t>
+          <t>H_ij_v[6,15,3]</t>
         </is>
       </c>
       <c r="B89" t="n">
@@ -1323,37 +1323,37 @@
     <row r="90">
       <c r="A90" s="1" t="inlineStr">
         <is>
-          <t>H_ij_v[7,17,3]</t>
+          <t>H_ij_v[8,10,5]</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="1" t="inlineStr">
         <is>
-          <t>H_ij_v[8,14,6]</t>
+          <t>H_ij_v[9,13,6]</t>
         </is>
       </c>
       <c r="B91" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="1" t="inlineStr">
         <is>
-          <t>H_ij_v[10,8,6]</t>
+          <t>H_ij_v[13,11,6]</t>
         </is>
       </c>
       <c r="B92" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="1" t="inlineStr">
         <is>
-          <t>H_ij_v[11,13,4]</t>
+          <t>H_ij_v[14,8,5]</t>
         </is>
       </c>
       <c r="B93" t="n">
@@ -1363,7 +1363,7 @@
     <row r="94">
       <c r="A94" s="1" t="inlineStr">
         <is>
-          <t>H_ij_v[12,16,5]</t>
+          <t>H_ij_v[15,17,3]</t>
         </is>
       </c>
       <c r="B94" t="n">
@@ -1373,7 +1373,7 @@
     <row r="95">
       <c r="A95" s="1" t="inlineStr">
         <is>
-          <t>H_ij_v[13,9,4]</t>
+          <t>H_ij_v[16,12,4]</t>
         </is>
       </c>
       <c r="B95" t="n">
@@ -1383,7 +1383,7 @@
     <row r="96">
       <c r="A96" s="1" t="inlineStr">
         <is>
-          <t>H_ij_v[16,18,5]</t>
+          <t>H_ij_v[17,7,3]</t>
         </is>
       </c>
       <c r="B96" t="n">
@@ -1393,221 +1393,111 @@
     <row r="97">
       <c r="A97" s="1" t="inlineStr">
         <is>
-          <t>H_ij_v[17,15,3]</t>
+          <t>H_ij_v[18,16,4]</t>
         </is>
       </c>
       <c r="B97" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="1" t="inlineStr">
         <is>
-          <t>G_i_t[3,1]</t>
+          <t>G_i_t[5,2]</t>
         </is>
       </c>
       <c r="B98" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="1" t="inlineStr">
         <is>
-          <t>G_i_t[3,2]</t>
+          <t>G_i_t[6,1]</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="1" t="inlineStr">
         <is>
-          <t>G_i_t[4,2]</t>
+          <t>G_i_v[7,3]</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>0.9999999999999989</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="1" t="inlineStr">
         <is>
-          <t>G_i_t[5,2]</t>
+          <t>G_i_v[8,5]</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>2.999999999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" s="1" t="inlineStr">
         <is>
-          <t>G_i_v[7,3]</t>
+          <t>G_i_v[10,5]</t>
         </is>
       </c>
       <c r="B102" t="n">
-        <v>11.00000000000001</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" s="1" t="inlineStr">
         <is>
-          <t>G_i_v[8,6]</t>
+          <t>G_i_v[11,6]</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="1" t="inlineStr">
         <is>
-          <t>G_i_v[9,4]</t>
+          <t>G_i_v[12,4]</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>1.999999999999996</v>
+        <v>2</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="1" t="inlineStr">
         <is>
-          <t>G_i_v[10,3]</t>
+          <t>G_i_v[13,6]</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="1" t="inlineStr">
         <is>
-          <t>G_i_v[12,3]</t>
+          <t>G_i_v[16,4]</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="1" t="inlineStr">
         <is>
-          <t>G_i_v[12,4]</t>
+          <t>G_i_v[17,3]</t>
         </is>
       </c>
       <c r="B107" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="108">
-      <c r="A108" s="1" t="inlineStr">
-        <is>
-          <t>G_i_v[13,3]</t>
-        </is>
-      </c>
-      <c r="B108" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="1" t="inlineStr">
-        <is>
-          <t>G_i_v[13,4]</t>
-        </is>
-      </c>
-      <c r="B109" t="n">
-        <v>0.9999999999999963</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="1" t="inlineStr">
-        <is>
-          <t>G_i_v[14,6]</t>
-        </is>
-      </c>
-      <c r="B110" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="1" t="inlineStr">
-        <is>
-          <t>G_i_v[15,3]</t>
-        </is>
-      </c>
-      <c r="B111" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="1" t="inlineStr">
-        <is>
-          <t>G_i_v[15,4]</t>
-        </is>
-      </c>
-      <c r="B112" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="1" t="inlineStr">
-        <is>
-          <t>G_i_v[15,5]</t>
-        </is>
-      </c>
-      <c r="B113" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="1" t="inlineStr">
-        <is>
-          <t>G_i_v[16,3]</t>
-        </is>
-      </c>
-      <c r="B114" t="n">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="115">
-      <c r="A115" s="1" t="inlineStr">
-        <is>
-          <t>G_i_v[16,5]</t>
-        </is>
-      </c>
-      <c r="B115" t="n">
-        <v>0.9999999999999961</v>
-      </c>
-    </row>
-    <row r="116">
-      <c r="A116" s="1" t="inlineStr">
-        <is>
-          <t>G_i_v[17,3]</t>
-        </is>
-      </c>
-      <c r="B116" t="n">
-        <v>12.00000000000001</v>
-      </c>
-    </row>
-    <row r="117">
-      <c r="A117" s="1" t="inlineStr">
-        <is>
-          <t>G_i_v[18,5]</t>
-        </is>
-      </c>
-      <c r="B117" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="118">
-      <c r="A118" s="1" t="inlineStr">
-        <is>
-          <t>G_i_v[20,3]</t>
-        </is>
-      </c>
-      <c r="B118" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>